<commit_message>
Update Excel data with latest changes
</commit_message>
<xml_diff>
--- a/public/data/MM_data.xlsx
+++ b/public/data/MM_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1509,16 +1509,16 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Palestine</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B66" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C66" t="str">
-        <v>Masjid-Al-Aqsa</v>
+        <v>Shwarmat</v>
       </c>
       <c r="D66" t="str">
-        <v>Baitul Muqaddas</v>
+        <v>Shawarma.</v>
       </c>
       <c r="E66" t="str">
         <v/>
@@ -1526,16 +1526,16 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B67" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C67" t="str">
-        <v>Shwarmat</v>
+        <v>Osma Perfumes</v>
       </c>
       <c r="D67" t="str">
-        <v>Shawarma.</v>
+        <v>Popular Madinah perfume shop. Premium perfumes.</v>
       </c>
       <c r="E67" t="str">
         <v/>
@@ -1543,16 +1543,16 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B68" t="str">
         <v>shopping</v>
       </c>
       <c r="C68" t="str">
-        <v>Osma Perfumes</v>
+        <v>ASQ Perfumes</v>
       </c>
       <c r="D68" t="str">
-        <v>Popular Madinah perfume shop. Premium perfumes.</v>
+        <v>Premium perfume store. Arabic &amp; Oud scents.</v>
       </c>
       <c r="E68" t="str">
         <v/>
@@ -1566,10 +1566,10 @@
         <v>shopping</v>
       </c>
       <c r="C69" t="str">
-        <v>ASQ Perfumes</v>
+        <v>Al Diyafa Mall</v>
       </c>
       <c r="D69" t="str">
-        <v>Premium perfume store. Arabic &amp; Oud scents.</v>
+        <v>Modern mall with dining.</v>
       </c>
       <c r="E69" t="str">
         <v/>
@@ -1577,16 +1577,16 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B70" t="str">
         <v>shopping</v>
       </c>
       <c r="C70" t="str">
-        <v>Al Diyafa Mall</v>
+        <v>Tamil Nadu Dates Shop</v>
       </c>
       <c r="D70" t="str">
-        <v>Modern mall with dining.</v>
+        <v>Shop No. 9, Near Gate 330 (Taiba Center side).</v>
       </c>
       <c r="E70" t="str">
         <v/>
@@ -1594,16 +1594,16 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B71" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C71" t="str">
-        <v>Tamil Nadu Dates Shop</v>
+        <v>Masjid al-Bilal</v>
       </c>
       <c r="D71" t="str">
-        <v>Shop No. 9, Near Gate 330 (Taiba Center side).</v>
+        <v>Landmark: Near Haram. Specialized for: Local prayer spot.</v>
       </c>
       <c r="E71" t="str">
         <v/>
@@ -1614,13 +1614,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B72" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C72" t="str">
-        <v>Masjid al-Bilal</v>
+        <v>Mama Ghazzel</v>
       </c>
       <c r="D72" t="str">
-        <v>Landmark: Near Haram. Specialized for: Local prayer spot.</v>
+        <v>Sweets &amp; desserts, Jabal E Omar area.</v>
       </c>
       <c r="E72" t="str">
         <v/>
@@ -1628,16 +1628,16 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B73" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C73" t="str">
-        <v>Mama Ghazzel</v>
+        <v>The International Fair &amp; Museum of the Prophet's Biography and Islamic Civilization</v>
       </c>
       <c r="D73" t="str">
-        <v>Sweets &amp; desserts, Jabal E Omar area.</v>
+        <v>Near Masjid an-Nabawi, immersive museum with VR, holography, and interactive displays.</v>
       </c>
       <c r="E73" t="str">
         <v/>
@@ -1648,13 +1648,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B74" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C74" t="str">
-        <v>The International Fair &amp; Museum of the Prophet's Biography and Islamic Civilization</v>
+        <v>Masjid Bilal Gold Market</v>
       </c>
       <c r="D74" t="str">
-        <v>Near Masjid an-Nabawi, immersive museum with VR, holography, and interactive displays.</v>
+        <v>Gate 5, gold jewelry.</v>
       </c>
       <c r="E74" t="str">
         <v/>
@@ -1665,13 +1665,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B75" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C75" t="str">
-        <v>Masjid Bilal Gold Market</v>
+        <v>Masjid Abu Bakr</v>
       </c>
       <c r="D75" t="str">
-        <v>Gate 5, gold jewelry.</v>
+        <v/>
       </c>
       <c r="E75" t="str">
         <v/>
@@ -1679,16 +1679,16 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B76" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C76" t="str">
-        <v>Masjid Abu Bakr</v>
+        <v>Thobes</v>
       </c>
       <c r="D76" t="str">
-        <v/>
+        <v>Aziziyah &amp; Misfalah shops - SAR 120 to 200.</v>
       </c>
       <c r="E76" t="str">
         <v/>
@@ -1702,10 +1702,10 @@
         <v>shopping</v>
       </c>
       <c r="C77" t="str">
-        <v>Thobes</v>
+        <v>Shamali Aziziya Mobile Market</v>
       </c>
       <c r="D77" t="str">
-        <v>Aziziyah &amp; Misfalah shops - SAR 120 to 200.</v>
+        <v>Cheap iPhones.</v>
       </c>
       <c r="E77" t="str">
         <v/>
@@ -1713,16 +1713,16 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B78" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C78" t="str">
-        <v>Shamali Aziziya Mobile Market</v>
+        <v>Masjid Ali</v>
       </c>
       <c r="D78" t="str">
-        <v>Cheap iPhones.</v>
+        <v/>
       </c>
       <c r="E78" t="str">
         <v/>
@@ -1733,13 +1733,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B79" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C79" t="str">
-        <v>Masjid Ali</v>
+        <v>Women's Abayas</v>
       </c>
       <c r="D79" t="str">
-        <v/>
+        <v>Gate 338, Grand Bazaar</v>
       </c>
       <c r="E79" t="str">
         <v/>
@@ -1747,16 +1747,16 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B80" t="str">
         <v>shopping</v>
       </c>
       <c r="C80" t="str">
-        <v>Women's Abayas</v>
+        <v>Ahmad Perfumes</v>
       </c>
       <c r="D80" t="str">
-        <v>Gate 338, Grand Bazaar</v>
+        <v>Popular Makkah perfume shop. Premium perfumes.</v>
       </c>
       <c r="E80" t="str">
         <v/>
@@ -1764,16 +1764,16 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>MAKKAH</v>
+        <v>JEDDAH</v>
       </c>
       <c r="B81" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C81" t="str">
-        <v>Ahmad Perfumes</v>
+        <v>Labash (Jeddah)</v>
       </c>
       <c r="D81" t="str">
-        <v>Popular Makkah perfume shop. Premium perfumes.</v>
+        <v>Modern grill restaurant.</v>
       </c>
       <c r="E81" t="str">
         <v/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>JEDDAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B82" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C82" t="str">
-        <v>Labash (Jeddah)</v>
+        <v>Ice Cream Al Asemah</v>
       </c>
       <c r="D82" t="str">
-        <v>Modern grill restaurant.</v>
+        <v>Off Al Ghufran Hotel, Ajyad Street (try Orange Slush, 10 SAR).</v>
       </c>
       <c r="E82" t="str">
         <v/>
@@ -1801,13 +1801,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B83" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C83" t="str">
-        <v>Ice Cream Al Asemah</v>
+        <v>Gabal Omar Mall</v>
       </c>
       <c r="D83" t="str">
-        <v>Off Al Ghufran Hotel, Ajyad Street (try Orange Slush, 10 SAR).</v>
+        <v>Mixed international brands.</v>
       </c>
       <c r="E83" t="str">
         <v/>
@@ -1818,13 +1818,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B84" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C84" t="str">
-        <v>Gabal Omar Mall</v>
+        <v>Masjid al-Haram</v>
       </c>
       <c r="D84" t="str">
-        <v>Mixed international brands.</v>
+        <v>Landmark: Clock Tower / Kaaba 0 km. Specialized for: Tawaf, Salah, Umrah &amp; Hajj. Tip: Visit early morning or late night to avoid crowds.</v>
       </c>
       <c r="E84" t="str">
         <v/>
@@ -1838,10 +1838,10 @@
         <v>places</v>
       </c>
       <c r="C85" t="str">
-        <v>Masjid al-Haram</v>
+        <v>Jannat al-Mu'alla Cemetery</v>
       </c>
       <c r="D85" t="str">
-        <v>Landmark: Clock Tower / Kaaba 0 km. Specialized for: Tawaf, Salah, Umrah &amp; Hajj. Tip: Visit early morning or late night to avoid crowds.</v>
+        <v>Distance: 1 km. Specialized for: Graves of Companions. Tip: Respectful visit.</v>
       </c>
       <c r="E85" t="str">
         <v/>
@@ -1849,16 +1849,16 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B86" t="str">
         <v>places</v>
       </c>
       <c r="C86" t="str">
-        <v>Jannat al-Mu'alla Cemetery</v>
+        <v>Bir al-Shifa Well</v>
       </c>
       <c r="D86" t="str">
-        <v>Distance: 1 km. Specialized for: Graves of Companions. Tip: Respectful visit.</v>
+        <v>80-100 km.</v>
       </c>
       <c r="E86" t="str">
         <v/>
@@ -1866,16 +1866,16 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B87" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C87" t="str">
-        <v>Bir al-Shifa Well</v>
+        <v>Dunkin Donuts Cold Brew</v>
       </c>
       <c r="D87" t="str">
-        <v>80-100 km.</v>
+        <v>Food to Try.</v>
       </c>
       <c r="E87" t="str">
         <v/>
@@ -1883,16 +1883,16 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B88" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C88" t="str">
-        <v>Dunkin Donuts Cold Brew</v>
+        <v>Uhud Mountain &amp; Martyrs' Cemetery</v>
       </c>
       <c r="D88" t="str">
-        <v>Food to Try.</v>
+        <v>6-7 km.</v>
       </c>
       <c r="E88" t="str">
         <v/>
@@ -1906,10 +1906,10 @@
         <v>places</v>
       </c>
       <c r="C89" t="str">
-        <v>Uhud Mountain &amp; Martyrs' Cemetery</v>
+        <v>Salman Farsi Garden / Masjid Salman al-Farsi</v>
       </c>
       <c r="D89" t="str">
-        <v>6-7 km.</v>
+        <v>4-7 km.</v>
       </c>
       <c r="E89" t="str">
         <v/>
@@ -1920,13 +1920,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B90" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C90" t="str">
-        <v>Salman Farsi Garden / Masjid Salman al-Farsi</v>
+        <v>Hakim Center</v>
       </c>
       <c r="D90" t="str">
-        <v>4-7 km.</v>
+        <v>Watches, Quba Street. Hakim Mall 2nd floor</v>
       </c>
       <c r="E90" t="str">
         <v/>
@@ -1934,16 +1934,16 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B91" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C91" t="str">
-        <v>Hakim Center</v>
+        <v>Masjid al-Ji'rana</v>
       </c>
       <c r="D91" t="str">
-        <v>Watches, Quba Street. Hakim Mall 2nd floor</v>
+        <v>Distance: 24-26 km. Specialized for: Miqat for locals / Miqat for residents of Makkah for Umrah, historic site after Battle of Hunayn.</v>
       </c>
       <c r="E91" t="str">
         <v/>
@@ -1957,10 +1957,10 @@
         <v>places</v>
       </c>
       <c r="C92" t="str">
-        <v>Masjid al-Ji'rana</v>
+        <v>House of Hazrat Abu Bakr Siddiq (RA)</v>
       </c>
       <c r="D92" t="str">
-        <v>Distance: 24-26 km. Specialized for: Miqat for locals / Miqat for residents of Makkah for Umrah, historic site after Battle of Hunayn.</v>
+        <v/>
       </c>
       <c r="E92" t="str">
         <v/>
@@ -1968,16 +1968,16 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B93" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C93" t="str">
-        <v>House of Hazrat Abu Bakr Siddiq (RA)</v>
+        <v>Ithmar Taiba Dates Company</v>
       </c>
       <c r="D93" t="str">
-        <v/>
+        <v>Premium dates &amp; gift packs. Ajwa dates.</v>
       </c>
       <c r="E93" t="str">
         <v/>
@@ -1988,13 +1988,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B94" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C94" t="str">
-        <v>Ithmar Taiba Dates Company</v>
+        <v>The Quba Walkway Park</v>
       </c>
       <c r="D94" t="str">
-        <v>Premium dates &amp; gift packs. Ajwa dates.</v>
+        <v>~4-5 km. 45-min scenic walk connecting Masjid an-Nabawi to Masjid Quba, lined with shops and resting spots.</v>
       </c>
       <c r="E94" t="str">
         <v/>
@@ -2002,16 +2002,16 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B95" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C95" t="str">
-        <v>The Quba Walkway Park</v>
+        <v>Authentic Arabic Shawarma (Crispyo Rolls)</v>
       </c>
       <c r="D95" t="str">
-        <v>~4-5 km. 45-min scenic walk connecting Masjid an-Nabawi to Masjid Quba, lined with shops and resting spots.</v>
+        <v>Clock Tower area, crisp rolls.</v>
       </c>
       <c r="E95" t="str">
         <v/>
@@ -2019,16 +2019,16 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B96" t="str">
         <v>food</v>
       </c>
       <c r="C96" t="str">
-        <v>Authentic Arabic Shawarma (Crispyo Rolls)</v>
+        <v>International Food Market</v>
       </c>
       <c r="D96" t="str">
-        <v>Clock Tower area, crisp rolls.</v>
+        <v>Ajwa Ice Cream.</v>
       </c>
       <c r="E96" t="str">
         <v/>
@@ -2036,16 +2036,16 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B97" t="str">
         <v>food</v>
       </c>
       <c r="C97" t="str">
-        <v>International Food Market</v>
+        <v>Qais Ice Cream</v>
       </c>
       <c r="D97" t="str">
-        <v>Ajwa Ice Cream.</v>
+        <v>Signature Saudi ice cream parlor. Ice cream &amp; local desserts.</v>
       </c>
       <c r="E97" t="str">
         <v/>
@@ -2053,16 +2053,16 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B98" t="str">
         <v>food</v>
       </c>
       <c r="C98" t="str">
-        <v>Qais Ice Cream</v>
+        <v>Abu Yasser Kitchen</v>
       </c>
       <c r="D98" t="str">
-        <v>Signature Saudi ice cream parlor. Ice cream &amp; local desserts.</v>
+        <v>Local Saudi dishes. Local Madinah food.</v>
       </c>
       <c r="E98" t="str">
         <v/>
@@ -2070,16 +2070,16 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B99" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C99" t="str">
-        <v>Abu Yasser Kitchen</v>
+        <v>Misfalah Market</v>
       </c>
       <c r="D99" t="str">
-        <v>Local Saudi dishes. Local Madinah food.</v>
+        <v>Budget abayas &amp; thobes.</v>
       </c>
       <c r="E99" t="str">
         <v/>
@@ -2090,13 +2090,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B100" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C100" t="str">
-        <v>Misfalah Market</v>
+        <v>Pakistani Restaurant #804</v>
       </c>
       <c r="D100" t="str">
-        <v>Budget abayas &amp; thobes.</v>
+        <v>Authentic Desi Breakfast.</v>
       </c>
       <c r="E100" t="str">
         <v/>
@@ -2107,13 +2107,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B101" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C101" t="str">
-        <v>Pakistani Restaurant #804</v>
+        <v>Bin Dawood (Aziziyah Branch)</v>
       </c>
       <c r="D101" t="str">
-        <v>Authentic Desi Breakfast.</v>
+        <v>Supermarket chain for groceries, clothes &amp; souvenirs. Groceries &amp; souvenirs, 3-4 km from Haram.</v>
       </c>
       <c r="E101" t="str">
         <v/>
@@ -2124,13 +2124,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B102" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C102" t="str">
-        <v>Bin Dawood (Aziziyah Branch)</v>
+        <v>Al Romansiah</v>
       </c>
       <c r="D102" t="str">
-        <v>Supermarket chain for groceries, clothes &amp; souvenirs. Groceries &amp; souvenirs, 3-4 km from Haram.</v>
+        <v>Chicken Mathgoot.</v>
       </c>
       <c r="E102" t="str">
         <v/>
@@ -2138,16 +2138,16 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B103" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C103" t="str">
-        <v>Al Romansiah</v>
+        <v>Masjid Quba</v>
       </c>
       <c r="D103" t="str">
-        <v>Chicken Mathgoot.</v>
+        <v>4-6 km, First mosque in Islam.</v>
       </c>
       <c r="E103" t="str">
         <v/>
@@ -2161,35 +2161,18 @@
         <v>places</v>
       </c>
       <c r="C104" t="str">
-        <v>Masjid Quba</v>
+        <v>Masjid Umar</v>
       </c>
       <c r="D104" t="str">
-        <v>4-6 km, First mosque in Islam.</v>
+        <v/>
       </c>
       <c r="E104" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="str">
-        <v>MADINAH</v>
-      </c>
-      <c r="B105" t="str">
-        <v>places</v>
-      </c>
-      <c r="C105" t="str">
-        <v>Masjid Umar</v>
-      </c>
-      <c r="D105" t="str">
-        <v/>
-      </c>
-      <c r="E105" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E105"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E104"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add edit name/details for all items and delete functionality (admin mode only)
</commit_message>
<xml_diff>
--- a/public/data/MM_data.xlsx
+++ b/public/data/MM_data.xlsx
@@ -424,13 +424,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B2" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C2" t="str">
-        <v>Farooji Express</v>
+        <v>Tailoring</v>
       </c>
       <c r="D2" t="str">
-        <v>Food to Try.</v>
+        <v>Daffah (Jabal Omar Makkah) and Al Shiaka (Jabal Omar &amp; Clock Tower Makkah)</v>
       </c>
       <c r="E2" t="str">
         <v/>
@@ -441,13 +441,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B3" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C3" t="str">
-        <v>Fastest Arrow Dates</v>
+        <v>The Quba Walkway Park</v>
       </c>
       <c r="D3" t="str">
-        <v>Premium dates, nuts, honey and chocolate. Very popular for premium real honey and high quality Ajwa dates</v>
+        <v>~4-5 km. 45-min scenic walk connecting Masjid an-Nabawi to Masjid Quba, lined with shops and resting spots.</v>
       </c>
       <c r="E3" t="str">
         <v/>
@@ -458,13 +458,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B4" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C4" t="str">
-        <v>Nimra Shinwari Hotel</v>
+        <v>Ahmad Perfumes</v>
       </c>
       <c r="D4" t="str">
-        <v>Peshawari Cuisine (Aziziya). Peshawari food, Aziziya.</v>
+        <v>Popular Makkah perfume shop. Premium perfumes.</v>
       </c>
       <c r="E4" t="str">
         <v/>
@@ -478,10 +478,10 @@
         <v>places</v>
       </c>
       <c r="C5" t="str">
-        <v>Masjid an-Nabawi</v>
+        <v>Companion Residences</v>
       </c>
       <c r="D5" t="str">
-        <v>Prophet's mosque, Central, Rawdah access/inside.</v>
+        <v>Near Quba area.</v>
       </c>
       <c r="E5" t="str">
         <v/>
@@ -489,16 +489,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B6" t="str">
         <v>shopping</v>
       </c>
       <c r="C6" t="str">
-        <v>Abraj Hypermarket</v>
+        <v>Bin Dawood (Madinah Branch)</v>
       </c>
       <c r="D6" t="str">
-        <v>Groceries &amp; souvenirs. General shopping.</v>
+        <v>Hypermarket near Masjid an-Nabawi.</v>
       </c>
       <c r="E6" t="str">
         <v/>
@@ -512,10 +512,10 @@
         <v>places</v>
       </c>
       <c r="C7" t="str">
-        <v>Al Ossia Bird Sanctuary</v>
+        <v>Masjid Abu Bakr</v>
       </c>
       <c r="D7" t="str">
-        <v>4-6 km.</v>
+        <v/>
       </c>
       <c r="E7" t="str">
         <v/>
@@ -523,16 +523,16 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B8" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C8" t="str">
-        <v>House of Sayyidah Fāțimah az-Zahra (RA)</v>
+        <v>Cut Fruit Salad</v>
       </c>
       <c r="D8" t="str">
-        <v>Within Masjid an-Nabawi, behind Rawdah.</v>
+        <v>From supermarkets / Random Supermarket. Food to Try.</v>
       </c>
       <c r="E8" t="str">
         <v/>
@@ -540,16 +540,16 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B9" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C9" t="str">
-        <v>Bin Dawood (Madinah Branch)</v>
+        <v>Monal Restaurant</v>
       </c>
       <c r="D9" t="str">
-        <v>Hypermarket near Masjid an-Nabawi.</v>
+        <v>Post-Umrah meals; highly rated.</v>
       </c>
       <c r="E9" t="str">
         <v/>
@@ -560,13 +560,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B10" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C10" t="str">
-        <v>Masjid al-Bilal</v>
+        <v>Lamsa Men's Tailor Shop</v>
       </c>
       <c r="D10" t="str">
-        <v>Near Quba, named after first muezzin. 4-6 km.</v>
+        <v>Custom thobes at affordable rates.</v>
       </c>
       <c r="E10" t="str">
         <v/>
@@ -577,13 +577,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B11" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C11" t="str">
-        <v>Al Dawoodiya (Mujamma Doodiya)</v>
+        <v>International Food Market</v>
       </c>
       <c r="D11" t="str">
-        <v>3 SAR shopping. Near Gate 310, moved to Al-Kakeh Building.</v>
+        <v>Ajwa Ice Cream.</v>
       </c>
       <c r="E11" t="str">
         <v/>
@@ -594,13 +594,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B12" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C12" t="str">
-        <v>Al Shurfa Al Alami Restaurant</v>
+        <v>ASQ Perfumes</v>
       </c>
       <c r="D12" t="str">
-        <v>Scenic view dining. Arabic cuisine.</v>
+        <v>Premium perfume store. Arabic &amp; Oud scents.</v>
       </c>
       <c r="E12" t="str">
         <v/>
@@ -608,16 +608,16 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B13" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C13" t="str">
-        <v>Almarai 100% Apple / Mixed Fruit Juice</v>
+        <v>Wateen 1 &amp; 2 Riyal Shop</v>
       </c>
       <c r="D13" t="str">
-        <v>(no sugar) Food to Try.</v>
+        <v>Budget gifts &amp; snacks. Gate 339</v>
       </c>
       <c r="E13" t="str">
         <v/>
@@ -628,13 +628,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B14" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C14" t="str">
-        <v>Wateen 1 &amp; 2 Riyal Shop</v>
+        <v>Masjid Umar</v>
       </c>
       <c r="D14" t="str">
-        <v>Budget gifts &amp; snacks. Gate 339</v>
+        <v/>
       </c>
       <c r="E14" t="str">
         <v/>
@@ -642,16 +642,16 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B15" t="str">
         <v>shopping</v>
       </c>
       <c r="C15" t="str">
-        <v>Tailoring</v>
+        <v>Women's Abayas</v>
       </c>
       <c r="D15" t="str">
-        <v>Custom thobes on Aziziyah Main Road available.</v>
+        <v>Souks near Masjid Quba &amp; Al Manakh area.</v>
       </c>
       <c r="E15" t="str">
         <v/>
@@ -662,13 +662,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B16" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C16" t="str">
-        <v>Abayas</v>
+        <v>Albaik</v>
       </c>
       <c r="D16" t="str">
-        <v>Ajyad, Misfalah &amp; Al Diyafa streets - SAR 40 to 100.</v>
+        <v>Broast chicken; near Haram; budget-friendly.</v>
       </c>
       <c r="E16" t="str">
         <v/>
@@ -676,16 +676,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B17" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C17" t="str">
-        <v>Karak Express</v>
+        <v>Masjid Ayesha (Tan'eem)</v>
       </c>
       <c r="D17" t="str">
-        <v>Chicken Biryani &amp; Karak Chai. Chai &amp; Chicken Biryani.</v>
+        <v>Miqat for Ihram, 7.5 km north of Kaaba. Tip: Taxi recommended.</v>
       </c>
       <c r="E17" t="str">
         <v/>
@@ -696,13 +696,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B18" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C18" t="str">
-        <v>Taiba Shopping</v>
+        <v>House of Sayyidah Fāțimah az-Zahra (RA)</v>
       </c>
       <c r="D18" t="str">
-        <v>Gate 331</v>
+        <v>Within Masjid an-Nabawi, behind Rawdah.</v>
       </c>
       <c r="E18" t="str">
         <v/>
@@ -713,13 +713,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B19" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C19" t="str">
-        <v>Barn's Coffee</v>
+        <v>House of Hazrat Abu Bakr Siddiq (RA)</v>
       </c>
       <c r="D19" t="str">
-        <v>Local Saudi coffee chain. Coffee &amp; snacks.</v>
+        <v/>
       </c>
       <c r="E19" t="str">
         <v/>
@@ -727,16 +727,16 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B20" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C20" t="str">
-        <v>Masjid Ayesha (Tan'eem)</v>
+        <v>Albaik</v>
       </c>
       <c r="D20" t="str">
-        <v>Miqat for Ihram, 7.5 km north of Kaaba. Tip: Taxi recommended.</v>
+        <v>Broast. Albaik style Broast.</v>
       </c>
       <c r="E20" t="str">
         <v/>
@@ -744,16 +744,16 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B21" t="str">
         <v>places</v>
       </c>
       <c r="C21" t="str">
-        <v>Masjid al-Jinn</v>
+        <v>Salman Farsi Garden / Masjid Salman al-Farsi</v>
       </c>
       <c r="D21" t="str">
-        <v>Distance: 1-3 km. Specialized for: Prophet recited Qur'an to jinn. Tip: Short visit, accessible by foot.</v>
+        <v>4-7 km.</v>
       </c>
       <c r="E21" t="str">
         <v/>
@@ -761,16 +761,16 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B22" t="str">
         <v>food</v>
       </c>
       <c r="C22" t="str">
-        <v>Gewar Taiba</v>
+        <v>Al Shurfa Al Alami Restaurant</v>
       </c>
       <c r="D22" t="str">
-        <v>Shawarma.</v>
+        <v>Scenic view dining. Arabic cuisine.</v>
       </c>
       <c r="E22" t="str">
         <v/>
@@ -784,27 +784,27 @@
         <v>places</v>
       </c>
       <c r="C23" t="str">
-        <v>Masjid al-Khandaq</v>
+        <v>Masjid an-Nabawi</v>
       </c>
       <c r="D23" t="str">
-        <v/>
+        <v>Prophet's mosque, Central, Rawdah access/inside.</v>
       </c>
       <c r="E23" t="str">
-        <v/>
+        <v>https://maps.app.goo.gl/e9V7NDbED5h4zbBJ6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B24" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C24" t="str">
-        <v>Any Local Shop</v>
+        <v>Masjid Bilal Gold Market</v>
       </c>
       <c r="D24" t="str">
-        <v>Shawarma with Rice.</v>
+        <v>Gate 5, gold jewelry.</v>
       </c>
       <c r="E24" t="str">
         <v/>
@@ -824,21 +824,21 @@
         <v>Site of Eid &amp; Istisqa prayers (western side of Masjid an-Nabawi).</v>
       </c>
       <c r="E25" t="str">
-        <v/>
+        <v>https://maps.app.goo.gl/RBiTxe4bAmWFWefe7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B26" t="str">
         <v>food</v>
       </c>
       <c r="C26" t="str">
-        <v>Fresh Lemonade</v>
+        <v>Al Safa Broast</v>
       </c>
       <c r="D26" t="str">
-        <v>@ Mount Arafat. Food to Try.</v>
+        <v>Madina Local Broast, better than Albaik, Gate 365</v>
       </c>
       <c r="E26" t="str">
         <v/>
@@ -846,16 +846,16 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B27" t="str">
         <v>food</v>
       </c>
       <c r="C27" t="str">
-        <v>Lamma Burger Crispy Roll / Red Burger</v>
+        <v>Kiffa Café</v>
       </c>
       <c r="D27" t="str">
-        <v>Food to Try.</v>
+        <v>Spanish Latte specialty drinks.</v>
       </c>
       <c r="E27" t="str">
         <v/>
@@ -866,13 +866,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B28" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C28" t="str">
-        <v>Mina / Muzdalifah / Mount Arafat</v>
+        <v>Khair Alzad Restaurant</v>
       </c>
       <c r="D28" t="str">
-        <v>Distance: 20-30 km. Specialized for: Hajj rituals. Tip: Arrange transport; not accessible for short Umrah visit.</v>
+        <v>Middle Eastern specialties, Abraj Al Bait Towers (next to STC).</v>
       </c>
       <c r="E28" t="str">
         <v/>
@@ -880,33 +880,33 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B29" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C29" t="str">
-        <v>Bofiya Safwa Al Juzum</v>
+        <v>Al Ossia Bird Sanctuary</v>
       </c>
       <c r="D29" t="str">
-        <v>Budget food spot in Alsafwah Markets. Budget meals.</v>
+        <v>4-6 km.</v>
       </c>
       <c r="E29" t="str">
-        <v/>
+        <v>https://maps.app.goo.gl/1iVAS2wu9cBQDbZL6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B30" t="str">
         <v>food</v>
       </c>
       <c r="C30" t="str">
-        <v>Qasr-ul-Amal Restaurant</v>
+        <v>Shwarmat</v>
       </c>
       <c r="D30" t="str">
-        <v>Traditional Arabic meals.</v>
+        <v>Shawarma.</v>
       </c>
       <c r="E30" t="str">
         <v/>
@@ -914,16 +914,16 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B31" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C31" t="str">
-        <v>Aliyat Al-Madinah Farms / Al Aliya Dates Farm</v>
+        <v>Thobes</v>
       </c>
       <c r="D31" t="str">
-        <v>10-20 km, Date Farm Experience.</v>
+        <v>Aziziyah &amp; Misfalah shops - SAR 120 to 200.</v>
       </c>
       <c r="E31" t="str">
         <v/>
@@ -931,16 +931,16 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B32" t="str">
         <v>places</v>
       </c>
       <c r="C32" t="str">
-        <v>Companion Residences</v>
+        <v>Kiswa Museum</v>
       </c>
       <c r="D32" t="str">
-        <v>Near Quba area.</v>
+        <v>Kiswa Museum near by Kiswa Factory (FAIHA)</v>
       </c>
       <c r="E32" t="str">
         <v/>
@@ -948,16 +948,16 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B33" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C33" t="str">
-        <v>Masjid al-Ghamamah</v>
+        <v>Al Dawoodiya (Mujamma Doodiya)</v>
       </c>
       <c r="D33" t="str">
-        <v>Landmark: Near Haram. Specialized for: Eid prayer &amp; historical significance. Historical mosque near Makkah (Eid &amp; Istisqa prayers).</v>
+        <v>3 SAR shopping. Near Gate 310, moved to Al-Kakeh Building.</v>
       </c>
       <c r="E33" t="str">
         <v/>
@@ -968,13 +968,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B34" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C34" t="str">
-        <v>Jabal al-Nour (Cave Hira)</v>
+        <v>Souk Al Khalil</v>
       </c>
       <c r="D34" t="str">
-        <v>Distance: Ash-Shafa 4-8 km. Specialized for: First revelation. Tip: Steep 1-2 hour climb; carry water &amp; wear shoes.</v>
+        <v>Traditional market behind Clock Tower.</v>
       </c>
       <c r="E34" t="str">
         <v/>
@@ -988,10 +988,10 @@
         <v>shopping</v>
       </c>
       <c r="C35" t="str">
-        <v>Souk Al Khalil</v>
+        <v>Gabal Omar Mall</v>
       </c>
       <c r="D35" t="str">
-        <v>Traditional market behind Clock Tower.</v>
+        <v>Mixed international brands.</v>
       </c>
       <c r="E35" t="str">
         <v/>
@@ -999,16 +999,16 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B36" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C36" t="str">
-        <v>Monal Restaurant</v>
+        <v>Osma Perfumes</v>
       </c>
       <c r="D36" t="str">
-        <v>Post-Umrah meals; highly rated.</v>
+        <v>Popular Madinah perfume shop. Premium perfumes.</v>
       </c>
       <c r="E36" t="str">
         <v/>
@@ -1019,13 +1019,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B37" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C37" t="str">
-        <v>Jamil's Restaurant</v>
+        <v>Bir al-Shifa Well</v>
       </c>
       <c r="D37" t="str">
-        <v>Desi Nashta (Halwa Puri, Paya, Paratha, Nihari). Desi breakfast.</v>
+        <v>80-100 km.</v>
       </c>
       <c r="E37" t="str">
         <v/>
@@ -1033,16 +1033,16 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B38" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C38" t="str">
-        <v>Turkish Station Underpass</v>
+        <v>Masjid al-Haram</v>
       </c>
       <c r="D38" t="str">
-        <v>Cheap local goods.</v>
+        <v>Landmark: Clock Tower / Kaaba 0 km. Specialized for: Tawaf, Salah, Umrah &amp; Hajj. Tip: Visit early morning or late night to avoid crowds.</v>
       </c>
       <c r="E38" t="str">
         <v/>
@@ -1053,13 +1053,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B39" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C39" t="str">
-        <v>Al Marwah Shop</v>
+        <v>Authentic Arabic Shawarma (Crispyo Rolls)</v>
       </c>
       <c r="D39" t="str">
-        <v>Cheapest gift shop in Makkah.</v>
+        <v>Clock Tower area, crisp rolls.</v>
       </c>
       <c r="E39" t="str">
         <v/>
@@ -1070,13 +1070,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B40" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C40" t="str">
-        <v>Kiswa Museum</v>
+        <v>Broast Al Farooj</v>
       </c>
       <c r="D40" t="str">
-        <v>Kiswa Museum near by Kiswa Factory (FAIHA)</v>
+        <v>Ibrahim Al Khalil Road.</v>
       </c>
       <c r="E40" t="str">
         <v/>
@@ -1087,13 +1087,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B41" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C41" t="str">
-        <v>Al Aziziyah Commercial Center</v>
+        <v>Al Tazaj</v>
       </c>
       <c r="D41" t="str">
-        <v>Fashion &amp; electronics.</v>
+        <v>Fried chicken; local chain.</v>
       </c>
       <c r="E41" t="str">
         <v/>
@@ -1107,10 +1107,10 @@
         <v>food</v>
       </c>
       <c r="C42" t="str">
-        <v>Nadec 100% Apple / Strawberry Juice</v>
+        <v>Zam Zam Café</v>
       </c>
       <c r="D42" t="str">
-        <v>Food to Try.</v>
+        <v>Chocolate Soufflé &amp; Ice Cream.</v>
       </c>
       <c r="E42" t="str">
         <v/>
@@ -1118,16 +1118,16 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B43" t="str">
         <v>food</v>
       </c>
       <c r="C43" t="str">
-        <v>Kiffa Café</v>
+        <v>Any Local Shop</v>
       </c>
       <c r="D43" t="str">
-        <v>Spanish Latte specialty drinks.</v>
+        <v>Shawarma with Rice.</v>
       </c>
       <c r="E43" t="str">
         <v/>
@@ -1135,16 +1135,16 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B44" t="str">
         <v>food</v>
       </c>
       <c r="C44" t="str">
-        <v>Albaik</v>
+        <v>Bofiya Safwa Al Juzum</v>
       </c>
       <c r="D44" t="str">
-        <v>Broast. Albaik style Broast.</v>
+        <v>Budget food spot in Alsafwah Markets. Budget meals.</v>
       </c>
       <c r="E44" t="str">
         <v/>
@@ -1152,16 +1152,16 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B45" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C45" t="str">
-        <v>Zam Zam Café</v>
+        <v>Taiba Shopping</v>
       </c>
       <c r="D45" t="str">
-        <v>Chocolate Soufflé &amp; Ice Cream.</v>
+        <v>Gate 331</v>
       </c>
       <c r="E45" t="str">
         <v/>
@@ -1172,13 +1172,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B46" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C46" t="str">
-        <v>Al Safa Broast</v>
+        <v>Wow 5 Mall</v>
       </c>
       <c r="D46" t="str">
-        <v>Madina Local Broast, better than Albaik, Gate 365</v>
+        <v>5 Riyal shop, Ali ibn Talib Road.</v>
       </c>
       <c r="E46" t="str">
         <v/>
@@ -1186,16 +1186,16 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B47" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C47" t="str">
-        <v>Premium Janimaz Shop</v>
+        <v>Masjid al-Ghamamah</v>
       </c>
       <c r="D47" t="str">
-        <v>Gate 305, prayer mats.</v>
+        <v>Landmark: Near Haram. Specialized for: Eid prayer &amp; historical significance. Historical mosque near Makkah (Eid &amp; Istisqa prayers).</v>
       </c>
       <c r="E47" t="str">
         <v/>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B48" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C48" t="str">
-        <v>Jabal al-Thawr (Cave Thawr)</v>
+        <v>Jamil's Restaurant</v>
       </c>
       <c r="D48" t="str">
-        <v>Distance: 7 km. Specialized for: Cave of Hijrah. Tip: Moderate hike; carry water.</v>
+        <v>Desi Nashta (Halwa Puri, Paya, Paratha, Nihari). Desi breakfast.</v>
       </c>
       <c r="E48" t="str">
         <v/>
@@ -1220,16 +1220,16 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B49" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C49" t="str">
-        <v>Khair Alzad Restaurant</v>
+        <v>Ithmar Taiba Dates Company</v>
       </c>
       <c r="D49" t="str">
-        <v>Middle Eastern specialties, Abraj Al Bait Towers (next to STC).</v>
+        <v>Premium dates &amp; gift packs. Ajwa dates.</v>
       </c>
       <c r="E49" t="str">
         <v/>
@@ -1237,16 +1237,16 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B50" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C50" t="str">
-        <v>Funduq Undlusia Restaurant</v>
+        <v>Hakim Center</v>
       </c>
       <c r="D50" t="str">
-        <v>Known for Arabic set meals. Local cuisine restaurant.</v>
+        <v>Watches, Quba Street. Hakim Mall 2nd floor</v>
       </c>
       <c r="E50" t="str">
         <v/>
@@ -1254,16 +1254,16 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B51" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C51" t="str">
-        <v>Masjid al-Fath</v>
+        <v>Al Aziziyah Commercial Center</v>
       </c>
       <c r="D51" t="str">
-        <v/>
+        <v>Fashion &amp; electronics.</v>
       </c>
       <c r="E51" t="str">
         <v/>
@@ -1271,16 +1271,16 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B52" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C52" t="str">
-        <v>Broast Al Farooj</v>
+        <v>Women's Abayas</v>
       </c>
       <c r="D52" t="str">
-        <v>Ibrahim Al Khalil Road.</v>
+        <v>Gate 338, Grand Bazaar</v>
       </c>
       <c r="E52" t="str">
         <v/>
@@ -1288,33 +1288,33 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>MADINAH</v>
+        <v>JEDDAH</v>
       </c>
       <c r="B53" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C53" t="str">
-        <v>Dawoodiya Market (Quba Road, Al Jumuah)</v>
+        <v>Labash (Jeddah)</v>
       </c>
       <c r="D53" t="str">
-        <v>Abayas from SAR 30 upwards.</v>
+        <v>Modern grill restaurant.</v>
       </c>
       <c r="E53" t="str">
-        <v/>
+        <v>https://maps.app.goo.gl/XhF8oYttEywBEu3k7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B54" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C54" t="str">
-        <v>Women's Abayas</v>
+        <v>Mina / Muzdalifah / Mount Arafat</v>
       </c>
       <c r="D54" t="str">
-        <v>Souks near Masjid Quba &amp; Al Manakh area.</v>
+        <v>Distance: 20-30 km. Specialized for: Hajj rituals. Tip: Arrange transport; not accessible for short Umrah visit.</v>
       </c>
       <c r="E54" t="str">
         <v/>
@@ -1322,16 +1322,16 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B55" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C55" t="str">
-        <v>Top 10 Shop (Aziziyah)</v>
+        <v>Masjid al-Qiblatain</v>
       </c>
       <c r="D55" t="str">
-        <v>Everything around 10 SAR (affordable gifts, toys, home items). Budget items (~10 SAR).</v>
+        <v>5-12 km, Qiblah change site/Where Qibla changed from Jerusalem to Makkah.</v>
       </c>
       <c r="E55" t="str">
         <v/>
@@ -1345,10 +1345,10 @@
         <v>food</v>
       </c>
       <c r="C56" t="str">
-        <v>Cut Fruit Salad</v>
+        <v>Pakistani Restaurant #804</v>
       </c>
       <c r="D56" t="str">
-        <v>From supermarkets / Random Supermarket. Food to Try.</v>
+        <v>Authentic Desi Breakfast.</v>
       </c>
       <c r="E56" t="str">
         <v/>
@@ -1356,16 +1356,16 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B57" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C57" t="str">
-        <v>Masjid al-Qiblatain</v>
+        <v>Fresh Lemonade</v>
       </c>
       <c r="D57" t="str">
-        <v>5-12 km, Qiblah change site/Where Qibla changed from Jerusalem to Makkah.</v>
+        <v>@ Mount Arafat. Food to Try.</v>
       </c>
       <c r="E57" t="str">
         <v/>
@@ -1373,16 +1373,16 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B58" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C58" t="str">
-        <v>Awaali Gardens</v>
+        <v>Tailoring</v>
       </c>
       <c r="D58" t="str">
-        <v>Historic palm groves gifted to Prophet.</v>
+        <v>Custom thobes on Aziziyah Main Road available.</v>
       </c>
       <c r="E58" t="str">
         <v/>
@@ -1393,13 +1393,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B59" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C59" t="str">
-        <v>Albaik</v>
+        <v>Al Diyafa Mall</v>
       </c>
       <c r="D59" t="str">
-        <v>Broast chicken; near Haram; budget-friendly.</v>
+        <v>Modern mall with dining.</v>
       </c>
       <c r="E59" t="str">
         <v/>
@@ -1410,13 +1410,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B60" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C60" t="str">
-        <v>Lamsa Men's Tailor Shop</v>
+        <v>Abu Yasser Kitchen</v>
       </c>
       <c r="D60" t="str">
-        <v>Custom thobes at affordable rates.</v>
+        <v>Local Saudi dishes. Local Madinah food.</v>
       </c>
       <c r="E60" t="str">
         <v/>
@@ -1427,16 +1427,16 @@
         <v>MADINAH</v>
       </c>
       <c r="B61" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C61" t="str">
-        <v>Wow 5 Mall</v>
+        <v>Aliyat Al-Madinah Farms / Al Aliya Dates Farm</v>
       </c>
       <c r="D61" t="str">
-        <v>5 Riyal shop, Ali ibn Talib Road.</v>
+        <v>10-20 km, Date Farm Experience.</v>
       </c>
       <c r="E61" t="str">
-        <v/>
+        <v>https://maps.app.goo.gl/1hVGw1iAXr1Eo8AK7</v>
       </c>
     </row>
     <row r="62">
@@ -1447,10 +1447,10 @@
         <v>shopping</v>
       </c>
       <c r="C62" t="str">
-        <v>Tailoring</v>
+        <v>Misfalah Market</v>
       </c>
       <c r="D62" t="str">
-        <v>Daffah (Jabal Omar Makkah) and Al Shiaka (Jabal Omar &amp; Clock Tower Makkah)</v>
+        <v>Budget abayas &amp; thobes.</v>
       </c>
       <c r="E62" t="str">
         <v/>
@@ -1464,10 +1464,10 @@
         <v>food</v>
       </c>
       <c r="C63" t="str">
-        <v>Al Tazaj</v>
+        <v>Qais Ice Cream</v>
       </c>
       <c r="D63" t="str">
-        <v>Fried chicken; local chain.</v>
+        <v>Signature Saudi ice cream parlor. Ice cream &amp; local desserts.</v>
       </c>
       <c r="E63" t="str">
         <v/>
@@ -1481,10 +1481,10 @@
         <v>places</v>
       </c>
       <c r="C64" t="str">
-        <v>Taif Day Trip</v>
+        <v>Jabal al-Thawr (Cave Thawr)</v>
       </c>
       <c r="D64" t="str">
-        <v>Distance: 90-95 km. Specialized for: Rose gardens &amp; markets, Rose distilleries &amp; mountain views. Tip: Day trip, best in morning.</v>
+        <v>Distance: 7 km. Specialized for: Cave of Hijrah. Tip: Moderate hike; carry water.</v>
       </c>
       <c r="E64" t="str">
         <v/>
@@ -1495,13 +1495,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B65" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C65" t="str">
-        <v>Ajyad Street Shops</v>
+        <v>Jabal al-Nour (Cave Hira)</v>
       </c>
       <c r="D65" t="str">
-        <v>Everyday wear &amp; scarves.</v>
+        <v>Distance: Ash-Shafa 4-8 km. Specialized for: First revelation. Tip: Steep 1-2 hour climb; carry water &amp; wear shoes.</v>
       </c>
       <c r="E65" t="str">
         <v/>
@@ -1512,13 +1512,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B66" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C66" t="str">
-        <v>Shwarmat</v>
+        <v>Ajyad Street Shops</v>
       </c>
       <c r="D66" t="str">
-        <v>Shawarma.</v>
+        <v>Everyday wear &amp; scarves.</v>
       </c>
       <c r="E66" t="str">
         <v/>
@@ -1526,16 +1526,16 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B67" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C67" t="str">
-        <v>Osma Perfumes</v>
+        <v>Al Romansiah</v>
       </c>
       <c r="D67" t="str">
-        <v>Popular Madinah perfume shop. Premium perfumes.</v>
+        <v>Chicken Mathgoot.</v>
       </c>
       <c r="E67" t="str">
         <v/>
@@ -1546,13 +1546,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B68" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C68" t="str">
-        <v>ASQ Perfumes</v>
+        <v>Jannat al-Mu'alla Cemetery</v>
       </c>
       <c r="D68" t="str">
-        <v>Premium perfume store. Arabic &amp; Oud scents.</v>
+        <v>Distance: 1 km. Specialized for: Graves of Companions. Tip: Respectful visit.</v>
       </c>
       <c r="E68" t="str">
         <v/>
@@ -1563,13 +1563,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B69" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C69" t="str">
-        <v>Al Diyafa Mall</v>
+        <v>Farooji Express</v>
       </c>
       <c r="D69" t="str">
-        <v>Modern mall with dining.</v>
+        <v>Food to Try.</v>
       </c>
       <c r="E69" t="str">
         <v/>
@@ -1580,16 +1580,16 @@
         <v>MADINAH</v>
       </c>
       <c r="B70" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C70" t="str">
-        <v>Tamil Nadu Dates Shop</v>
+        <v>Masjid al-Fath</v>
       </c>
       <c r="D70" t="str">
-        <v>Shop No. 9, Near Gate 330 (Taiba Center side).</v>
+        <v/>
       </c>
       <c r="E70" t="str">
-        <v/>
+        <v>https://maps.app.goo.gl/1GjnwkmbeyMybBmg8</v>
       </c>
     </row>
     <row r="71">
@@ -1611,16 +1611,16 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B72" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C72" t="str">
-        <v>Mama Ghazzel</v>
+        <v>Masjid Ali</v>
       </c>
       <c r="D72" t="str">
-        <v>Sweets &amp; desserts, Jabal E Omar area.</v>
+        <v/>
       </c>
       <c r="E72" t="str">
         <v/>
@@ -1631,13 +1631,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B73" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C73" t="str">
-        <v>The International Fair &amp; Museum of the Prophet's Biography and Islamic Civilization</v>
+        <v>Fastest Arrow Dates</v>
       </c>
       <c r="D73" t="str">
-        <v>Near Masjid an-Nabawi, immersive museum with VR, holography, and interactive displays.</v>
+        <v>Premium dates, nuts, honey and chocolate. Very popular for premium real honey and high quality Ajwa dates</v>
       </c>
       <c r="E73" t="str">
         <v/>
@@ -1651,10 +1651,10 @@
         <v>shopping</v>
       </c>
       <c r="C74" t="str">
-        <v>Masjid Bilal Gold Market</v>
+        <v>Turkish Station Underpass</v>
       </c>
       <c r="D74" t="str">
-        <v>Gate 5, gold jewelry.</v>
+        <v>Cheap local goods.</v>
       </c>
       <c r="E74" t="str">
         <v/>
@@ -1662,16 +1662,16 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B75" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C75" t="str">
-        <v>Masjid Abu Bakr</v>
+        <v>Al Marwah Shop</v>
       </c>
       <c r="D75" t="str">
-        <v/>
+        <v>Cheapest gift shop in Makkah.</v>
       </c>
       <c r="E75" t="str">
         <v/>
@@ -1685,10 +1685,10 @@
         <v>shopping</v>
       </c>
       <c r="C76" t="str">
-        <v>Thobes</v>
+        <v>Bin Dawood (Aziziyah Branch)</v>
       </c>
       <c r="D76" t="str">
-        <v>Aziziyah &amp; Misfalah shops - SAR 120 to 200.</v>
+        <v>Supermarket chain for groceries, clothes &amp; souvenirs. Groceries &amp; souvenirs, 3-4 km from Haram.</v>
       </c>
       <c r="E76" t="str">
         <v/>
@@ -1702,10 +1702,10 @@
         <v>shopping</v>
       </c>
       <c r="C77" t="str">
-        <v>Shamali Aziziya Mobile Market</v>
+        <v>Top 10 Shop (Aziziyah)</v>
       </c>
       <c r="D77" t="str">
-        <v>Cheap iPhones.</v>
+        <v>Everything around 10 SAR (affordable gifts, toys, home items). Budget items (~10 SAR).</v>
       </c>
       <c r="E77" t="str">
         <v/>
@@ -1716,13 +1716,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B78" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C78" t="str">
-        <v>Masjid Ali</v>
+        <v>Gewar Taiba</v>
       </c>
       <c r="D78" t="str">
-        <v/>
+        <v>Shawarma.</v>
       </c>
       <c r="E78" t="str">
         <v/>
@@ -1733,13 +1733,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B79" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C79" t="str">
-        <v>Women's Abayas</v>
+        <v>The International Fair &amp; Museum of the Prophet's Biography and Islamic Civilization</v>
       </c>
       <c r="D79" t="str">
-        <v>Gate 338, Grand Bazaar</v>
+        <v>Near Masjid an-Nabawi, immersive museum with VR, holography, and interactive displays.</v>
       </c>
       <c r="E79" t="str">
         <v/>
@@ -1750,13 +1750,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B80" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C80" t="str">
-        <v>Ahmad Perfumes</v>
+        <v>Mama Ghazzel</v>
       </c>
       <c r="D80" t="str">
-        <v>Popular Makkah perfume shop. Premium perfumes.</v>
+        <v>Sweets &amp; desserts, Jabal E Omar area.</v>
       </c>
       <c r="E80" t="str">
         <v/>
@@ -1764,16 +1764,16 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>JEDDAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B81" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C81" t="str">
-        <v>Labash (Jeddah)</v>
+        <v>Lamma Burger Crispy Roll / Red Burger</v>
       </c>
       <c r="D81" t="str">
-        <v>Modern grill restaurant.</v>
+        <v>Food to Try.</v>
       </c>
       <c r="E81" t="str">
         <v/>
@@ -1787,10 +1787,10 @@
         <v>food</v>
       </c>
       <c r="C82" t="str">
-        <v>Ice Cream Al Asemah</v>
+        <v>Nimra Shinwari Hotel</v>
       </c>
       <c r="D82" t="str">
-        <v>Off Al Ghufran Hotel, Ajyad Street (try Orange Slush, 10 SAR).</v>
+        <v>Peshawari Cuisine (Aziziya). Peshawari food, Aziziya.</v>
       </c>
       <c r="E82" t="str">
         <v/>
@@ -1804,10 +1804,10 @@
         <v>shopping</v>
       </c>
       <c r="C83" t="str">
-        <v>Gabal Omar Mall</v>
+        <v>Abayas</v>
       </c>
       <c r="D83" t="str">
-        <v>Mixed international brands.</v>
+        <v>Ajyad, Misfalah &amp; Al Diyafa streets - SAR 40 to 100.</v>
       </c>
       <c r="E83" t="str">
         <v/>
@@ -1818,13 +1818,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B84" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C84" t="str">
-        <v>Masjid al-Haram</v>
+        <v>Ice Cream Al Asemah</v>
       </c>
       <c r="D84" t="str">
-        <v>Landmark: Clock Tower / Kaaba 0 km. Specialized for: Tawaf, Salah, Umrah &amp; Hajj. Tip: Visit early morning or late night to avoid crowds.</v>
+        <v>Off Al Ghufran Hotel, Ajyad Street (try Orange Slush, 10 SAR).</v>
       </c>
       <c r="E84" t="str">
         <v/>
@@ -1838,10 +1838,10 @@
         <v>places</v>
       </c>
       <c r="C85" t="str">
-        <v>Jannat al-Mu'alla Cemetery</v>
+        <v>Masjid al-Jinn</v>
       </c>
       <c r="D85" t="str">
-        <v>Distance: 1 km. Specialized for: Graves of Companions. Tip: Respectful visit.</v>
+        <v>Distance: 1-3 km. Specialized for: Prophet recited Qur'an to jinn. Tip: Short visit, accessible by foot.</v>
       </c>
       <c r="E85" t="str">
         <v/>
@@ -1852,13 +1852,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B86" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C86" t="str">
-        <v>Bir al-Shifa Well</v>
+        <v>Dawoodiya Market (Quba Road, Al Jumuah)</v>
       </c>
       <c r="D86" t="str">
-        <v>80-100 km.</v>
+        <v>Abayas from SAR 30 upwards.</v>
       </c>
       <c r="E86" t="str">
         <v/>
@@ -1866,16 +1866,16 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B87" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C87" t="str">
-        <v>Dunkin Donuts Cold Brew</v>
+        <v>Uhud Mountain &amp; Martyrs' Cemetery</v>
       </c>
       <c r="D87" t="str">
-        <v>Food to Try.</v>
+        <v>6-7 km.</v>
       </c>
       <c r="E87" t="str">
         <v/>
@@ -1889,27 +1889,27 @@
         <v>places</v>
       </c>
       <c r="C88" t="str">
-        <v>Uhud Mountain &amp; Martyrs' Cemetery</v>
+        <v>Masjid al-Bilal</v>
       </c>
       <c r="D88" t="str">
-        <v>6-7 km.</v>
+        <v>Near Quba, named after first muezzin. 4-6 km.</v>
       </c>
       <c r="E88" t="str">
-        <v/>
+        <v>https://maps.app.goo.gl/67eRWTuV7jhwLa5J9</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B89" t="str">
         <v>places</v>
       </c>
       <c r="C89" t="str">
-        <v>Salman Farsi Garden / Masjid Salman al-Farsi</v>
+        <v>Taif Day Trip</v>
       </c>
       <c r="D89" t="str">
-        <v>4-7 km.</v>
+        <v>Distance: 90-95 km. Specialized for: Rose gardens &amp; markets, Rose distilleries &amp; mountain views. Tip: Day trip, best in morning.</v>
       </c>
       <c r="E89" t="str">
         <v/>
@@ -1917,16 +1917,16 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B90" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C90" t="str">
-        <v>Hakim Center</v>
+        <v>Barn's Coffee</v>
       </c>
       <c r="D90" t="str">
-        <v>Watches, Quba Street. Hakim Mall 2nd floor</v>
+        <v>Local Saudi coffee chain. Coffee &amp; snacks.</v>
       </c>
       <c r="E90" t="str">
         <v/>
@@ -1937,13 +1937,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B91" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C91" t="str">
-        <v>Masjid al-Ji'rana</v>
+        <v>Almarai 100% Apple / Mixed Fruit Juice</v>
       </c>
       <c r="D91" t="str">
-        <v>Distance: 24-26 km. Specialized for: Miqat for locals / Miqat for residents of Makkah for Umrah, historic site after Battle of Hunayn.</v>
+        <v>(no sugar) Food to Try.</v>
       </c>
       <c r="E91" t="str">
         <v/>
@@ -1954,13 +1954,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B92" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C92" t="str">
-        <v>House of Hazrat Abu Bakr Siddiq (RA)</v>
+        <v>Abraj Hypermarket</v>
       </c>
       <c r="D92" t="str">
-        <v/>
+        <v>Groceries &amp; souvenirs. General shopping.</v>
       </c>
       <c r="E92" t="str">
         <v/>
@@ -1968,16 +1968,16 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B93" t="str">
-        <v>shopping</v>
+        <v>food</v>
       </c>
       <c r="C93" t="str">
-        <v>Ithmar Taiba Dates Company</v>
+        <v>Funduq Undlusia Restaurant</v>
       </c>
       <c r="D93" t="str">
-        <v>Premium dates &amp; gift packs. Ajwa dates.</v>
+        <v>Known for Arabic set meals. Local cuisine restaurant.</v>
       </c>
       <c r="E93" t="str">
         <v/>
@@ -1988,13 +1988,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B94" t="str">
-        <v>places</v>
+        <v>shopping</v>
       </c>
       <c r="C94" t="str">
-        <v>The Quba Walkway Park</v>
+        <v>Premium Janimaz Shop</v>
       </c>
       <c r="D94" t="str">
-        <v>~4-5 km. 45-min scenic walk connecting Masjid an-Nabawi to Masjid Quba, lined with shops and resting spots.</v>
+        <v>Gate 305, prayer mats.</v>
       </c>
       <c r="E94" t="str">
         <v/>
@@ -2002,16 +2002,16 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B95" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C95" t="str">
-        <v>Authentic Arabic Shawarma (Crispyo Rolls)</v>
+        <v>Masjid Quba</v>
       </c>
       <c r="D95" t="str">
-        <v>Clock Tower area, crisp rolls.</v>
+        <v>4-6 km, First mosque in Islam.</v>
       </c>
       <c r="E95" t="str">
         <v/>
@@ -2025,10 +2025,10 @@
         <v>food</v>
       </c>
       <c r="C96" t="str">
-        <v>International Food Market</v>
+        <v>Karak Express</v>
       </c>
       <c r="D96" t="str">
-        <v>Ajwa Ice Cream.</v>
+        <v>Chicken Biryani &amp; Karak Chai. Chai &amp; Chicken Biryani.</v>
       </c>
       <c r="E96" t="str">
         <v/>
@@ -2039,13 +2039,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B97" t="str">
-        <v>food</v>
+        <v>shopping</v>
       </c>
       <c r="C97" t="str">
-        <v>Qais Ice Cream</v>
+        <v>Shamali Aziziya Mobile Market</v>
       </c>
       <c r="D97" t="str">
-        <v>Signature Saudi ice cream parlor. Ice cream &amp; local desserts.</v>
+        <v>Cheap iPhones.</v>
       </c>
       <c r="E97" t="str">
         <v/>
@@ -2053,16 +2053,16 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>MADINAH</v>
+        <v>MAKKAH</v>
       </c>
       <c r="B98" t="str">
         <v>food</v>
       </c>
       <c r="C98" t="str">
-        <v>Abu Yasser Kitchen</v>
+        <v>Dunkin Donuts Cold Brew</v>
       </c>
       <c r="D98" t="str">
-        <v>Local Saudi dishes. Local Madinah food.</v>
+        <v>Food to Try.</v>
       </c>
       <c r="E98" t="str">
         <v/>
@@ -2070,16 +2070,16 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B99" t="str">
-        <v>shopping</v>
+        <v>places</v>
       </c>
       <c r="C99" t="str">
-        <v>Misfalah Market</v>
+        <v>Awaali Gardens</v>
       </c>
       <c r="D99" t="str">
-        <v>Budget abayas &amp; thobes.</v>
+        <v>Historic palm groves gifted to Prophet.</v>
       </c>
       <c r="E99" t="str">
         <v/>
@@ -2090,13 +2090,13 @@
         <v>MAKKAH</v>
       </c>
       <c r="B100" t="str">
-        <v>food</v>
+        <v>places</v>
       </c>
       <c r="C100" t="str">
-        <v>Pakistani Restaurant #804</v>
+        <v>Masjid al-Ji'rana</v>
       </c>
       <c r="D100" t="str">
-        <v>Authentic Desi Breakfast.</v>
+        <v>Distance: 24-26 km. Specialized for: Miqat for locals / Miqat for residents of Makkah for Umrah, historic site after Battle of Hunayn.</v>
       </c>
       <c r="E100" t="str">
         <v/>
@@ -2104,16 +2104,16 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>MAKKAH</v>
+        <v>MADINAH</v>
       </c>
       <c r="B101" t="str">
         <v>shopping</v>
       </c>
       <c r="C101" t="str">
-        <v>Bin Dawood (Aziziyah Branch)</v>
+        <v>Tamil Nadu Dates Shop</v>
       </c>
       <c r="D101" t="str">
-        <v>Supermarket chain for groceries, clothes &amp; souvenirs. Groceries &amp; souvenirs, 3-4 km from Haram.</v>
+        <v>Shop No. 9, Near Gate 330 (Taiba Center side).</v>
       </c>
       <c r="E101" t="str">
         <v/>
@@ -2127,10 +2127,10 @@
         <v>food</v>
       </c>
       <c r="C102" t="str">
-        <v>Al Romansiah</v>
+        <v>Nadec 100% Apple / Strawberry Juice</v>
       </c>
       <c r="D102" t="str">
-        <v>Chicken Mathgoot.</v>
+        <v>Food to Try.</v>
       </c>
       <c r="E102" t="str">
         <v/>
@@ -2141,13 +2141,13 @@
         <v>MADINAH</v>
       </c>
       <c r="B103" t="str">
-        <v>places</v>
+        <v>food</v>
       </c>
       <c r="C103" t="str">
-        <v>Masjid Quba</v>
+        <v>Qasr-ul-Amal Restaurant</v>
       </c>
       <c r="D103" t="str">
-        <v>4-6 km, First mosque in Islam.</v>
+        <v>Traditional Arabic meals.</v>
       </c>
       <c r="E103" t="str">
         <v/>
@@ -2161,7 +2161,7 @@
         <v>places</v>
       </c>
       <c r="C104" t="str">
-        <v>Masjid Umar</v>
+        <v>Masjid al-Khandaq</v>
       </c>
       <c r="D104" t="str">
         <v/>

</xml_diff>

<commit_message>
Fix Excel parser to read SortOrder/IsPinned/IsAdminAdded and UI improvements
- Fix Excel parser to read SortOrder, IsPinned, IsAdminAdded from Excel columns instead of ignoring them
- Add fallback to auto-numbering if columns don't exist
- Fix dark mode compatibility in debug page (status messages and tip box)
- Fix header icon alignment (Info, Theme toggle, Settings now on same line)
- Improve mobile category tabs fit with responsive sizing (xs/sm/md breakpoints)
- Reduce mobile tab padding and font size for better fit on small screens
</commit_message>
<xml_diff>
--- a/public/data/MM_data.xlsx
+++ b/public/data/MM_data.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nsyed3/Workspace/Local/Private/MM_App/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530D788A-BA31-E549-8FC8-D58B671724A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1CD56F-EC4E-6C4B-94AD-DCF936BE4C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="680" windowWidth="28360" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29560" yWindow="-340" windowWidth="38080" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$109</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="254">
   <si>
     <t>City</t>
   </si>
@@ -760,12 +760,6 @@
     <t>Dunkin Donuts Cold Brew</t>
   </si>
   <si>
-    <t>Awaali Gardens</t>
-  </si>
-  <si>
-    <t>Historic palm groves gifted to Prophet.</t>
-  </si>
-  <si>
     <t>Masjid al-Ji'rana</t>
   </si>
   <si>
@@ -791,6 +785,18 @@
   </si>
   <si>
     <t>https://maps.app.goo.gl/v5VCu6RXfo1xmvQk9</t>
+  </si>
+  <si>
+    <t>Etrah Garden</t>
+  </si>
+  <si>
+    <t>Ajwatech</t>
+  </si>
+  <si>
+    <t>Saraya Ward Restaurant</t>
+  </si>
+  <si>
+    <t>Reef al-Maknan</t>
   </si>
 </sst>
 </file>
@@ -1167,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="S114" sqref="S114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1248,7 +1254,7 @@
         <v>15</v>
       </c>
       <c r="K2">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="L2" t="s">
         <v>19</v>
@@ -1289,7 +1295,7 @@
         <v>15</v>
       </c>
       <c r="K3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3" t="s">
         <v>19</v>
@@ -1330,7 +1336,7 @@
         <v>15</v>
       </c>
       <c r="K4">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
         <v>19</v>
@@ -1371,7 +1377,7 @@
         <v>15</v>
       </c>
       <c r="K5">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L5" t="s">
         <v>19</v>
@@ -1412,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="K6">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
         <v>19</v>
@@ -1453,7 +1459,7 @@
         <v>15</v>
       </c>
       <c r="K7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L7" t="s">
         <v>19</v>
@@ -1494,7 +1500,7 @@
         <v>15</v>
       </c>
       <c r="K8">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="L8" t="s">
         <v>19</v>
@@ -1535,7 +1541,7 @@
         <v>15</v>
       </c>
       <c r="K9">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L9" t="s">
         <v>19</v>
@@ -1576,7 +1582,7 @@
         <v>15</v>
       </c>
       <c r="K10">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="L10" t="s">
         <v>19</v>
@@ -1617,7 +1623,7 @@
         <v>15</v>
       </c>
       <c r="K11">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="L11" t="s">
         <v>19</v>
@@ -1658,7 +1664,7 @@
         <v>15</v>
       </c>
       <c r="K12">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="L12" t="s">
         <v>19</v>
@@ -1699,7 +1705,7 @@
         <v>15</v>
       </c>
       <c r="K13">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="L13" t="s">
         <v>19</v>
@@ -1740,7 +1746,7 @@
         <v>15</v>
       </c>
       <c r="K14">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L14" t="s">
         <v>19</v>
@@ -1781,7 +1787,7 @@
         <v>15</v>
       </c>
       <c r="K15">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="L15" t="s">
         <v>19</v>
@@ -1822,7 +1828,7 @@
         <v>15</v>
       </c>
       <c r="K16">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="L16" t="s">
         <v>19</v>
@@ -1863,7 +1869,7 @@
         <v>15</v>
       </c>
       <c r="K17">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="L17" t="s">
         <v>19</v>
@@ -1904,7 +1910,7 @@
         <v>15</v>
       </c>
       <c r="K18">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="L18" t="s">
         <v>19</v>
@@ -1945,7 +1951,7 @@
         <v>15</v>
       </c>
       <c r="K19">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="L19" t="s">
         <v>19</v>
@@ -1986,7 +1992,7 @@
         <v>15</v>
       </c>
       <c r="K20">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L20" t="s">
         <v>19</v>
@@ -2027,7 +2033,7 @@
         <v>15</v>
       </c>
       <c r="K21">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="L21" t="s">
         <v>19</v>
@@ -2068,7 +2074,7 @@
         <v>15</v>
       </c>
       <c r="K22">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="L22" t="s">
         <v>19</v>
@@ -2109,7 +2115,7 @@
         <v>15</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" t="s">
         <v>70</v>
@@ -2150,7 +2156,7 @@
         <v>15</v>
       </c>
       <c r="K24">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="L24" t="s">
         <v>19</v>
@@ -2191,7 +2197,7 @@
         <v>15</v>
       </c>
       <c r="K25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L25" t="s">
         <v>19</v>
@@ -2232,7 +2238,7 @@
         <v>15</v>
       </c>
       <c r="K26">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L26" t="s">
         <v>19</v>
@@ -2314,7 +2320,7 @@
         <v>15</v>
       </c>
       <c r="K28">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="L28" t="s">
         <v>19</v>
@@ -2355,7 +2361,7 @@
         <v>15</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="L29" t="s">
         <v>19</v>
@@ -2396,7 +2402,7 @@
         <v>15</v>
       </c>
       <c r="K30">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="L30" t="s">
         <v>19</v>
@@ -2437,7 +2443,7 @@
         <v>15</v>
       </c>
       <c r="K31">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="L31" t="s">
         <v>19</v>
@@ -2478,7 +2484,7 @@
         <v>15</v>
       </c>
       <c r="K32">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="L32" t="s">
         <v>19</v>
@@ -2519,7 +2525,7 @@
         <v>15</v>
       </c>
       <c r="K33">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="L33" t="s">
         <v>19</v>
@@ -2560,7 +2566,7 @@
         <v>15</v>
       </c>
       <c r="K34">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L34" t="s">
         <v>19</v>
@@ -2601,7 +2607,7 @@
         <v>15</v>
       </c>
       <c r="K35">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="L35" t="s">
         <v>19</v>
@@ -2642,7 +2648,7 @@
         <v>15</v>
       </c>
       <c r="K36">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="L36" t="s">
         <v>19</v>
@@ -2683,7 +2689,7 @@
         <v>15</v>
       </c>
       <c r="K37">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L37" t="s">
         <v>19</v>
@@ -2724,7 +2730,7 @@
         <v>15</v>
       </c>
       <c r="K38">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="L38" t="s">
         <v>70</v>
@@ -2765,7 +2771,7 @@
         <v>15</v>
       </c>
       <c r="K39">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="L39" t="s">
         <v>19</v>
@@ -2806,7 +2812,7 @@
         <v>15</v>
       </c>
       <c r="K40">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="L40" t="s">
         <v>19</v>
@@ -2847,7 +2853,7 @@
         <v>15</v>
       </c>
       <c r="K41">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="L41" t="s">
         <v>19</v>
@@ -2888,7 +2894,7 @@
         <v>15</v>
       </c>
       <c r="K42">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L42" t="s">
         <v>19</v>
@@ -2929,7 +2935,7 @@
         <v>15</v>
       </c>
       <c r="K43">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="L43" t="s">
         <v>19</v>
@@ -2970,7 +2976,7 @@
         <v>15</v>
       </c>
       <c r="K44">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="L44" t="s">
         <v>19</v>
@@ -3011,7 +3017,7 @@
         <v>15</v>
       </c>
       <c r="K45">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="L45" t="s">
         <v>19</v>
@@ -3052,7 +3058,7 @@
         <v>15</v>
       </c>
       <c r="K46">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="L46" t="s">
         <v>19</v>
@@ -3093,7 +3099,7 @@
         <v>15</v>
       </c>
       <c r="K47">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="L47" t="s">
         <v>19</v>
@@ -3134,7 +3140,7 @@
         <v>15</v>
       </c>
       <c r="K48">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="L48" t="s">
         <v>19</v>
@@ -3175,7 +3181,7 @@
         <v>15</v>
       </c>
       <c r="K49">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="L49" t="s">
         <v>19</v>
@@ -3216,7 +3222,7 @@
         <v>15</v>
       </c>
       <c r="K50">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="L50" t="s">
         <v>19</v>
@@ -3257,7 +3263,7 @@
         <v>15</v>
       </c>
       <c r="K51">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="L51" t="s">
         <v>19</v>
@@ -3298,7 +3304,7 @@
         <v>15</v>
       </c>
       <c r="K52">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="L52" t="s">
         <v>19</v>
@@ -3336,7 +3342,7 @@
         <v>15</v>
       </c>
       <c r="K53">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="L53" t="s">
         <v>19</v>
@@ -3377,7 +3383,7 @@
         <v>15</v>
       </c>
       <c r="K54">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="L54" t="s">
         <v>19</v>
@@ -3418,7 +3424,7 @@
         <v>15</v>
       </c>
       <c r="K55">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="L55" t="s">
         <v>19</v>
@@ -3459,7 +3465,7 @@
         <v>15</v>
       </c>
       <c r="K56">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="L56" t="s">
         <v>19</v>
@@ -3500,7 +3506,7 @@
         <v>15</v>
       </c>
       <c r="K57">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="L57" t="s">
         <v>19</v>
@@ -3541,7 +3547,7 @@
         <v>15</v>
       </c>
       <c r="K58">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="L58" t="s">
         <v>19</v>
@@ -3579,7 +3585,7 @@
         <v>15</v>
       </c>
       <c r="K59">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="L59" t="s">
         <v>19</v>
@@ -3620,7 +3626,7 @@
         <v>15</v>
       </c>
       <c r="K60">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="L60" t="s">
         <v>19</v>
@@ -3661,7 +3667,7 @@
         <v>15</v>
       </c>
       <c r="K61">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="L61" t="s">
         <v>19</v>
@@ -3702,7 +3708,7 @@
         <v>15</v>
       </c>
       <c r="K62">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="L62" t="s">
         <v>19</v>
@@ -3743,7 +3749,7 @@
         <v>15</v>
       </c>
       <c r="K63">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="L63" t="s">
         <v>19</v>
@@ -3784,7 +3790,7 @@
         <v>15</v>
       </c>
       <c r="K64">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="L64" t="s">
         <v>19</v>
@@ -3825,7 +3831,7 @@
         <v>15</v>
       </c>
       <c r="K65">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="L65" t="s">
         <v>19</v>
@@ -3866,7 +3872,7 @@
         <v>15</v>
       </c>
       <c r="K66">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="L66" t="s">
         <v>19</v>
@@ -3907,7 +3913,7 @@
         <v>15</v>
       </c>
       <c r="K67">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="L67" t="s">
         <v>19</v>
@@ -3948,7 +3954,7 @@
         <v>15</v>
       </c>
       <c r="K68">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="L68" t="s">
         <v>19</v>
@@ -3989,7 +3995,7 @@
         <v>15</v>
       </c>
       <c r="K69">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="L69" t="s">
         <v>19</v>
@@ -4030,7 +4036,7 @@
         <v>15</v>
       </c>
       <c r="K70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L70" t="s">
         <v>19</v>
@@ -4071,7 +4077,7 @@
         <v>15</v>
       </c>
       <c r="K71">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="L71" t="s">
         <v>19</v>
@@ -4112,7 +4118,7 @@
         <v>15</v>
       </c>
       <c r="K72">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L72" t="s">
         <v>19</v>
@@ -4153,7 +4159,7 @@
         <v>15</v>
       </c>
       <c r="K73">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="L73" t="s">
         <v>19</v>
@@ -4194,7 +4200,7 @@
         <v>15</v>
       </c>
       <c r="K74">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="L74" t="s">
         <v>19</v>
@@ -4235,7 +4241,7 @@
         <v>15</v>
       </c>
       <c r="K75">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="L75" t="s">
         <v>19</v>
@@ -4317,7 +4323,7 @@
         <v>15</v>
       </c>
       <c r="K77">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="L77" t="s">
         <v>19</v>
@@ -4358,7 +4364,7 @@
         <v>15</v>
       </c>
       <c r="K78">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="L78" t="s">
         <v>19</v>
@@ -4399,7 +4405,7 @@
         <v>15</v>
       </c>
       <c r="K79">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="L79" t="s">
         <v>19</v>
@@ -4440,7 +4446,7 @@
         <v>15</v>
       </c>
       <c r="K80">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="L80" t="s">
         <v>19</v>
@@ -4481,7 +4487,7 @@
         <v>15</v>
       </c>
       <c r="K81">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="L81" t="s">
         <v>19</v>
@@ -4522,7 +4528,7 @@
         <v>15</v>
       </c>
       <c r="K82">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="L82" t="s">
         <v>19</v>
@@ -4563,7 +4569,7 @@
         <v>15</v>
       </c>
       <c r="K83">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="L83" t="s">
         <v>19</v>
@@ -4604,7 +4610,7 @@
         <v>15</v>
       </c>
       <c r="K84">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="L84" t="s">
         <v>19</v>
@@ -4645,7 +4651,7 @@
         <v>15</v>
       </c>
       <c r="K85">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L85" t="s">
         <v>19</v>
@@ -4686,7 +4692,7 @@
         <v>15</v>
       </c>
       <c r="K86">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="L86" t="s">
         <v>19</v>
@@ -4727,7 +4733,7 @@
         <v>15</v>
       </c>
       <c r="K87">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="L87" t="s">
         <v>19</v>
@@ -4768,7 +4774,7 @@
         <v>15</v>
       </c>
       <c r="K88">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="L88" t="s">
         <v>19</v>
@@ -4809,7 +4815,7 @@
         <v>15</v>
       </c>
       <c r="K89">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="L89" t="s">
         <v>19</v>
@@ -4850,7 +4856,7 @@
         <v>15</v>
       </c>
       <c r="K90">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L90" t="s">
         <v>19</v>
@@ -4891,7 +4897,7 @@
         <v>15</v>
       </c>
       <c r="K91">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="L91" t="s">
         <v>19</v>
@@ -4932,7 +4938,7 @@
         <v>15</v>
       </c>
       <c r="K92">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="L92" t="s">
         <v>19</v>
@@ -4973,7 +4979,7 @@
         <v>15</v>
       </c>
       <c r="K93">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="L93" t="s">
         <v>19</v>
@@ -5014,7 +5020,7 @@
         <v>15</v>
       </c>
       <c r="K94">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="L94" t="s">
         <v>19</v>
@@ -5055,7 +5061,7 @@
         <v>15</v>
       </c>
       <c r="K95">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="L95" t="s">
         <v>19</v>
@@ -5096,7 +5102,7 @@
         <v>15</v>
       </c>
       <c r="K96">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="L96" t="s">
         <v>19</v>
@@ -5137,7 +5143,7 @@
         <v>15</v>
       </c>
       <c r="K97">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="L97" t="s">
         <v>19</v>
@@ -5178,7 +5184,7 @@
         <v>15</v>
       </c>
       <c r="K98">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="L98" t="s">
         <v>19</v>
@@ -5219,7 +5225,7 @@
         <v>15</v>
       </c>
       <c r="K99">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="L99" t="s">
         <v>19</v>
@@ -5260,7 +5266,7 @@
         <v>15</v>
       </c>
       <c r="K100">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="L100" t="s">
         <v>19</v>
@@ -5280,10 +5286,7 @@
         <v>181</v>
       </c>
       <c r="D101" t="s">
-        <v>241</v>
-      </c>
-      <c r="E101" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="F101" t="s">
         <v>15</v>
@@ -5301,7 +5304,7 @@
         <v>15</v>
       </c>
       <c r="K101">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="L101" t="s">
         <v>19</v>
@@ -5321,10 +5324,10 @@
         <v>177</v>
       </c>
       <c r="D102" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E102" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F102" t="s">
         <v>15</v>
@@ -5342,7 +5345,7 @@
         <v>15</v>
       </c>
       <c r="K102">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="L102" t="s">
         <v>19</v>
@@ -5362,10 +5365,10 @@
         <v>15</v>
       </c>
       <c r="D103" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E103" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F103" t="s">
         <v>15</v>
@@ -5383,7 +5386,7 @@
         <v>15</v>
       </c>
       <c r="K103">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="L103" t="s">
         <v>19</v>
@@ -5403,7 +5406,7 @@
         <v>15</v>
       </c>
       <c r="D104" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E104" t="s">
         <v>170</v>
@@ -5424,7 +5427,7 @@
         <v>15</v>
       </c>
       <c r="K104">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="L104" t="s">
         <v>19</v>
@@ -5444,10 +5447,10 @@
         <v>15</v>
       </c>
       <c r="D105" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E105" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F105" t="s">
         <v>15</v>
@@ -5465,7 +5468,7 @@
         <v>15</v>
       </c>
       <c r="K105">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="L105" t="s">
         <v>19</v>
@@ -5485,13 +5488,13 @@
         <v>177</v>
       </c>
       <c r="D106" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E106" t="s">
         <v>15</v>
       </c>
       <c r="F106" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G106" t="s">
         <v>18</v>
@@ -5515,11 +5518,117 @@
         <v>19</v>
       </c>
     </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>20</v>
+      </c>
+      <c r="B107" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107" t="s">
+        <v>253</v>
+      </c>
+      <c r="F107" t="s">
+        <v>15</v>
+      </c>
+      <c r="G107" t="s">
+        <v>18</v>
+      </c>
+      <c r="H107" t="s">
+        <v>15</v>
+      </c>
+      <c r="I107" t="s">
+        <v>15</v>
+      </c>
+      <c r="J107" t="s">
+        <v>15</v>
+      </c>
+      <c r="K107">
+        <v>50</v>
+      </c>
+      <c r="L107" t="s">
+        <v>19</v>
+      </c>
+      <c r="M107" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108" t="s">
+        <v>33</v>
+      </c>
+      <c r="D108" t="s">
+        <v>252</v>
+      </c>
+      <c r="F108" t="s">
+        <v>15</v>
+      </c>
+      <c r="G108" t="s">
+        <v>18</v>
+      </c>
+      <c r="H108" t="s">
+        <v>15</v>
+      </c>
+      <c r="I108" t="s">
+        <v>15</v>
+      </c>
+      <c r="J108" t="s">
+        <v>15</v>
+      </c>
+      <c r="K108">
+        <v>49</v>
+      </c>
+      <c r="L108" t="s">
+        <v>19</v>
+      </c>
+      <c r="M108" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>20</v>
+      </c>
+      <c r="B109" t="s">
+        <v>33</v>
+      </c>
+      <c r="D109" t="s">
+        <v>251</v>
+      </c>
+      <c r="F109" t="s">
+        <v>15</v>
+      </c>
+      <c r="G109" t="s">
+        <v>18</v>
+      </c>
+      <c r="H109" t="s">
+        <v>15</v>
+      </c>
+      <c r="I109" t="s">
+        <v>15</v>
+      </c>
+      <c r="J109" t="s">
+        <v>15</v>
+      </c>
+      <c r="K109">
+        <v>51</v>
+      </c>
+      <c r="L109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M109" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M106" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M109" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:M6 A54:M54 A53 D53:M53 A8:M13 A7:B7 D7:M7 A15:M16 A14:B14 D14:M14 A18:M20 A17:B17 D17:M17 A24:M24 A23:B23 D23:M23 A26:M28 A25:B25 D25:M25 A39:M46 A38:B38 D38:M38 A48:M52 A47:B47 D47:M47 A56:M58 A55:B55 D55:M55 A73:M86 A70:B70 D70:M70 A71:B71 D71:M71 A72:B72 D72:M72 A88:M89 A87:B87 D87:M87 A91:M96 A90:B90 D90:M90 A98:M100 A97:B97 D97:M97 A103:M105 A102:B102 D102:M102 A106:B106 D106:M106 A101:B101 D101:M101 A62:M69 A61:B61 D61:M61 A30:M37 A29:B29 D29:M29 A22:M22 A21:B21 D21:M21 A60:M60 A59:B59 D59:M59" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:M1 A54:J54 A53 D53:J53 A11:J11 A7:B7 D7:J7 A15:J15 A14:B14 D14:J14 A18:J18 A17:B17 D17:J17 A24:J24 A23:B23 D23:J23 A27:M27 A25:B25 D25:J25 A46:J46 A38:B38 D38:J38 A48:J48 A47:B47 D47:J47 A57:J57 A55:B55 D55:J55 A76:M76 A70:B70 D70:J70 A71:B71 D71:J71 A72:B72 D72:J72 A88:J88 A87:B87 D87:J87 A93:J93 A90:B90 D90:J90 A98:J98 A97:B97 D97:J97 A103:J103 A102:B102 D102:J102 A106:B106 D106:M106 A101:B101 F101:J101 A63:J63 A61:B61 D61:J61 A30:J30 A29:B29 D29:J29 A22:J22 A21:B21 D21:J21 A60:J60 A59:B59 D59:J59 L17:M17 L38:M38 L47:M47 L71:M71 L87:M87 L102:M102 A33:J33 A31:J31 L31:M31 A58:J58 L58:M58 A62:J62 L62:M62 A86:J86 A85:J85 L85:M85 A20:J20 A19:J19 L19:M19 A32:J32 L32:M32 L54:M54 A67:J67 A64:J64 L64:M64 A65:J65 L65:M65 A69:J69 A68:J68 L68:M68 A91:J91 L91:M91 A3:J3 A2:J2 L2:M2 A6:J6 A4:J4 L4:M4 A13:J13 A12:J12 L12:M12 A36:J36 A34:J34 L34:M34 A35:J35 L35:M35 A52:J52 A51:J51 L51:M51 L59:M59 A66:J66 L66:M66 A80:J80 A77:J77 L77:M77 A78:J78 L78:M78 A79:J79 L79:M79 A96:J96 A94:J94 L94:M94 A100:J100 A99:J99 L99:M99 A8:J8 L8:M8 A9:J9 L9:M9 A16:J16 L16:M16 L22:M22 A28:J28 L28:M28 L30:M30 A39:J39 L39:M39 A40:J40 L40:M40 A41:J41 L41:M41 A42:J42 L42:M42 A43:J43 L43:M43 A44:J44 L44:M44 A56:J56 L56:M56 L57:M57 L63:M63 L67:M67 L69:M69 A84:J84 A82:J82 L82:M82 A83:J83 L83:M83 L84:M84 L86:M86 A92:J92 L92:M92 L93:M93 A95:J95 L95:M95 L100:M100 A105:J105 A104:J104 L104:M104 L23:M23 L97:M97 L7:M7 L14:M14 L25:M25 L55:M55 L90:M90 L70:M70 L72:M72 A73:J73 L73:M73 L101:M101 L21:M21 L29:M29 L61:M61 A74:J74 L74:M74 L3:M3 A5:J5 L5:M5 L18:M18 A37:J37 L37:M37 A81:J81 L81:M81 A89:J89 L89:M89 A10:J10 L10:M10 L15:M15 L88:M88 L52:M52 L6:M6 L13:M13 L24:M24 L33:M33 L36:M36 A45:J45 L45:M45 L46:M46 A50:J50 A49:J49 L49:M49 L50:M50 A75:J75 L75:M75 L96:M96 L103:M103 L20:M20 A26:J26 L26:M26 L80:M80 L98:M98 L48:M48 L60:M60 L11:M11 L105:M105 L53:M53" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>